<commit_message>
tech_route, tech_promos, promos: added [products], [promo_values].
</commit_message>
<xml_diff>
--- a/htdocs/assets/promos.xlsx
+++ b/htdocs/assets/promos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -70,7 +70,13 @@
     <t xml:space="preserve">Бренд</t>
   </si>
   <si>
-    <t xml:space="preserve">Вид промо активности</t>
+    <t xml:space="preserve">Продукт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вид промо механики</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Детали промо механики</t>
   </si>
   <si>
     <t xml:space="preserve">Фото</t>
@@ -107,6 +113,12 @@
   </si>
   <si>
     <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
   </si>
 </sst>
 </file>
@@ -115,11 +127,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -162,6 +174,12 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -227,7 +245,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +286,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,6 +299,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,18 +387,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N3" activeCellId="0" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -392,14 +418,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="39.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="18" style="4" width="5.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="27.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="24" style="5" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="66" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="4" width="31.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="20" style="4" width="5.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="27.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="67" min="26" style="5" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="68" style="6" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="9"/>
@@ -416,156 +444,171 @@
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12" t="s">
+      <c r="S2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="T2" s="13" t="s">
         <v>19</v>
+      </c>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="13" t="n">
+      <c r="C3" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="H3" s="14" t="n">
+      <c r="H3" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="I3" s="14" t="n">
+      <c r="I3" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="J3" s="14" t="n">
+      <c r="J3" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="14" t="n">
+      <c r="K3" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="L3" s="14" t="n">
+      <c r="L3" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="M3" s="14" t="n">
+      <c r="M3" s="16" t="n">
         <v>13</v>
       </c>
-      <c r="N3" s="14" t="n">
+      <c r="N3" s="16" t="n">
         <v>14</v>
       </c>
-      <c r="O3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="14" t="s">
+      <c r="O3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="P3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="Q3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="R3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="S3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="T3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="14" t="s">
+      <c r="U3" s="16" t="s">
         <v>28</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="T2:W2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>